<commit_message>
Tests sur le clone qui roule. Ajout du drivetrain et des fonctions de manette.
</commit_message>
<xml_diff>
--- a/first2019 planification systemes.xlsx
+++ b/first2019 planification systemes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\503003453\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fenix\workspace\robot2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E7B69FB5-636F-40BF-83E4-28396015C7C0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF8312B-140C-4527-8D5A-EC75EC22A101}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14910" windowHeight="7215" xr2:uid="{2B0AB050-5AE3-4731-8730-7E0C92F268C1}"/>
+    <workbookView minimized="1" xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8964" xr2:uid="{2B0AB050-5AE3-4731-8730-7E0C92F268C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -324,17 +324,17 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -367,7 +367,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -666,20 +666,20 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -696,8 +696,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B2" t="s">
@@ -716,8 +716,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -731,11 +731,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B5" t="s">
@@ -754,8 +754,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>14</v>
       </c>
@@ -763,23 +763,23 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
       <c r="C7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4"/>
       <c r="C8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B10" t="s">
@@ -798,8 +798,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>37</v>
       </c>
@@ -816,8 +816,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>38</v>
       </c>
@@ -834,8 +834,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>39</v>
       </c>
@@ -852,8 +852,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
       <c r="C14" t="s">
         <v>45</v>
       </c>
@@ -864,8 +864,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
       <c r="C15" t="s">
         <v>46</v>
       </c>
@@ -873,37 +873,37 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
       <c r="D16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
       <c r="D17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
       <c r="B22" t="s">
         <v>48</v>
       </c>
@@ -911,8 +911,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
       <c r="B23" t="s">
         <v>49</v>
       </c>
@@ -920,8 +920,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
       <c r="B24" t="s">
         <v>50</v>
       </c>
@@ -929,8 +929,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
       <c r="B25" t="s">
         <v>51</v>
       </c>
@@ -938,14 +938,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="5"/>
+    </row>
+    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B28" t="s">
@@ -955,8 +955,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
       <c r="B29" t="s">
         <v>60</v>
       </c>
@@ -964,8 +964,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
       <c r="B30" t="s">
         <v>3</v>
       </c>
@@ -973,8 +973,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
       <c r="B31" t="s">
         <v>64</v>
       </c>
@@ -982,8 +982,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -994,8 +994,9 @@
     <mergeCell ref="A28:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>